<commit_message>
Refactoring project so it can be used with JGrasp as well as STS / IntelliJ
</commit_message>
<xml_diff>
--- a/src/main/LightPatterns.xlsx
+++ b/src/main/LightPatterns.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Nate\java_tools\Workspaces\SchoolWorkspace\ChristmasTreePi\src\main\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A07B5E56-D96C-4CA4-ACBC-C336BC8928CC}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FA8D07B-9E05-4CAD-9B5D-BD688104D132}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" activeTab="3" xr2:uid="{A15E4088-1328-44C0-9881-D69A13DB1AD9}"/>
   </bookViews>
@@ -309,9 +309,9 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -647,21 +647,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="E1" s="5" t="s">
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="E1" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="I1" s="5" t="s">
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="I1" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -992,21 +992,21 @@
       </c>
     </row>
     <row r="20" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A20" s="5" t="s">
+      <c r="A20" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
-      <c r="E20" s="5" t="s">
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
+      <c r="E20" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="F20" s="6"/>
-      <c r="G20" s="6"/>
-      <c r="I20" s="5" t="s">
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+      <c r="I20" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="J20" s="6"/>
-      <c r="K20" s="6"/>
+      <c r="J20" s="7"/>
+      <c r="K20" s="7"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
@@ -1397,21 +1397,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="E1" s="5" t="s">
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="E1" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="I1" s="5" t="s">
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="I1" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -1675,21 +1675,21 @@
       </c>
     </row>
     <row r="20" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A20" s="5" t="s">
+      <c r="A20" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
-      <c r="E20" s="5" t="s">
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
+      <c r="E20" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F20" s="6"/>
-      <c r="G20" s="6"/>
-      <c r="I20" s="5" t="s">
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+      <c r="I20" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="J20" s="6"/>
-      <c r="K20" s="6"/>
+      <c r="J20" s="7"/>
+      <c r="K20" s="7"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
@@ -1921,7 +1921,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7744E465-51CF-4402-ACE1-B294179E562F}">
-  <dimension ref="A1:K246"/>
+  <dimension ref="A1:I246"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
@@ -2487,7 +2487,7 @@
       <c r="B37" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C37" s="7" t="s">
+      <c r="C37" s="5" t="s">
         <v>32</v>
       </c>
       <c r="D37" s="1" t="s">

</xml_diff>